<commit_message>
2nd time trying to commit
</commit_message>
<xml_diff>
--- a/hosted_files/QREST/QREST-Sending to AQS.xlsx
+++ b/hosted_files/QREST/QREST-Sending to AQS.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melinda\Dropbox (NAU Research)\QREST-Team\QREST-PublicToShare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melinda\Documents\GitHub\tamscenter.github.io\hosted_files\QREST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CF81B70-4A08-4B65-AF2F-EC05E8E587E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8451489E-D428-4A8E-9ECA-E7FC68123D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-1850" windowWidth="19420" windowHeight="10560" xr2:uid="{7715871D-8683-4309-BD27-314EA3A9CF8F}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{7715871D-8683-4309-BD27-314EA3A9CF8F}"/>
   </bookViews>
   <sheets>
-    <sheet name="A.SubmittalSetup" sheetId="4" r:id="rId1"/>
-    <sheet name="B.MonitoringData" sheetId="7" r:id="rId2"/>
-    <sheet name="C. QC Data" sheetId="8" r:id="rId3"/>
-    <sheet name="References" sheetId="5" r:id="rId4"/>
+    <sheet name="QREST-setup" sheetId="4" r:id="rId1"/>
+    <sheet name="1timeAQSsetup" sheetId="9" r:id="rId2"/>
+    <sheet name="DataSelection" sheetId="7" r:id="rId3"/>
+    <sheet name="QC Data" sheetId="8" r:id="rId4"/>
+    <sheet name="References" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId6"/>
+    <sheet name="scraps" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
   <si>
     <t>SOP:</t>
   </si>
@@ -172,33 +175,6 @@
   </si>
   <si>
     <t>AQS Manuals and References from the USEPA, Mike King, and Navajo Nation EPA:</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Verify that the AQS user ID and the AQS Screening Group Name are correct.  The Screening Group name must be exactly the same as how AQS lists  your screening group.  (Also, what AQS lists as your Screening Group is sometimes not </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <u/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>exactly</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> what AQS lists as your Agency name.  Access AQS and/or your EPA AQS contact person to verify your Screening Group name; see References.)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">This opens a panel listing all previous AQS files generated in QREST for your agency.  Click Add.  </t>
@@ -314,6 +290,226 @@
   <si>
     <t xml:space="preserve">It is likely that the email address corresponding to the AQS user name will receive an email from AQS before the status of the submittal is refreshed in QREST.  Check for those emails, but eventually the status of the submittal in QREST will receive the information from AQS with the status as Pending, Processing, Completed or Error, similar to the Refresh button in AQS.  The emails sent by AQS to the email associated with this AQS ID (such as ROE) often provide information needed to diagnose any problems.  </t>
   </si>
+  <si>
+    <r>
+      <t>Configuring your pipeline to AQS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:  There are several once-and-done steps to set up QREST so that your data get appended to the right files in AQS.  This configuration only needs to be done once, and the only </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>requirement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is that the person sending the data to AQS have an account that is associated with your tribal agency, listed by AQS as a "screening group."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>AQS User Account:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The user must have an EPA AQS account with Screening Group access. If you do not already have one, the user must contact EPA’s AQS program to obtain an AQS account (https://www.epa.gov/aqs, or just search online for "us epa aqs.") </t>
+    </r>
+  </si>
+  <si>
+    <t>The exact name of the screening group in AQS may be slightly different than the Tribal Agency name.  For example, our Tribal Air Monitoring Support Center has Agency code 1262, with the name as shown, but our AQS Screening Group is "ITEP Training." </t>
+  </si>
+  <si>
+    <t>Log into AQS using your account.  Note that when you send data to AQS, the email that AQS has for this account will receive emails about the status of your data submittal. </t>
+  </si>
+  <si>
+    <t>When you log in, AQS will ask you if you are a read-only user or have access to a screening group. </t>
+  </si>
+  <si>
+    <t>When you select Screening Group Access, AQS will then show you what screening groups you are associated with:</t>
+  </si>
+  <si>
+    <t>Note the exact spelling of this Screening Group, because it must be entered in QREST</t>
+  </si>
+  <si>
+    <r>
+      <t>Screening Group</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:  It is critical to get the name of your screening group exactly as AQS spells it, so that QREST can be correctly configured to send data to your site in AQS. </t>
+    </r>
+  </si>
+  <si>
+    <t>After logging into AQS, navigate to Admin -&gt; Security:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Save </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the record in AQS.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Configure QREST to send from your account</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>In QREST, navigate to Air Data -&gt; AQS Submission page.</t>
+    </r>
+  </si>
+  <si>
+    <t>Click the Add button (at the bottom of a list of previous AQS submissions), then select the Site you wish to submit for (if you are working with more than one site).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On the right side box it lists the credentials that QREST will use to make the AQS submission. Click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Change </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>button to setup these credentials or to change them:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Once you click the Change button, the AQS Submission Accounts page opens.  Enter your AQS User ID and the name of your screening group, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">exactly </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as it was shown when you logged into AQS</t>
+    </r>
+  </si>
+  <si>
+    <t>and selected Screening Group Access:</t>
+  </si>
+  <si>
+    <t>If you want to use QREST's global CDX account (the account of the TAMS Center's QREST Admin), then check that box:</t>
+  </si>
+  <si>
+    <t>If you want to use your own EN (CDX) credentials, then the EN user name and password must be entered in QREST, and importantly, entered in AQS's Admin-&gt; Security page as described above.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the AQS user ID and the AQS Screening Group Name are correct.  The Screening Group name must be exactly the same as how AQS lists  your screening group.  (Also, what AQS lists as your Screening Group is sometimes not </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exactly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> what AQS lists as your Agency name.  Access AQS and/or your EPA AQS contact person to verify your Screening Group name; see References and 1timeAQSsetup.)</t>
+    </r>
+  </si>
+  <si>
+    <t>The AQS Security page opens.  Leave all the information as is (unless it is not accurate), except replace the EN Account with the EN account you want to use.  If you wish, you can use QREST's admin account, which is MELINDA.RONCA-BATTISTA@NAU.EDU (all caps).</t>
+  </si>
 </sst>
 </file>
 
@@ -322,7 +518,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -414,6 +610,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -472,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -515,6 +777,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -539,14 +811,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -560,7 +832,21 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -893,8 +1179,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="443796" y="6850240"/>
-          <a:ext cx="5698770" cy="1293238"/>
+          <a:off x="435329" y="7015340"/>
+          <a:ext cx="5449004" cy="1322872"/>
           <a:chOff x="449793" y="7143751"/>
           <a:chExt cx="5688540" cy="1293944"/>
         </a:xfrm>
@@ -1850,6 +2136,316 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>60325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>231775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57F02C98-F07E-18F7-330C-2B6A882BCCD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="60325" y="2066925"/>
+          <a:ext cx="4667250" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>377825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>29237</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8441A2B2-C953-339A-E3F4-28743928EEB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3730625"/>
+          <a:ext cx="2308225" cy="829337"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>260349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>302578</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>212724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4599437-E37F-AB8A-0BF3-63AA5A4F32D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="79375" y="4791074"/>
+          <a:ext cx="2153603" cy="733425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>325438</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>250032</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>857251</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>10004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{413830B3-5E39-B46B-EEF8-11F90CEC0B27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="325438" y="6377782"/>
+          <a:ext cx="3425032" cy="2379347"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>146843</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>31388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>317239</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>3969</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE1451E-E46A-4B8F-8475-BAAE5942262E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="146843" y="9564326"/>
+          <a:ext cx="2099209" cy="1282268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>273050</xdr:colOff>
       <xdr:row>10</xdr:row>
@@ -2107,8 +2703,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="545770" y="7104954"/>
-          <a:ext cx="7142710" cy="1285643"/>
+          <a:off x="531762" y="7282380"/>
+          <a:ext cx="6783189" cy="1318327"/>
           <a:chOff x="548341" y="7711263"/>
           <a:chExt cx="7103869" cy="1303914"/>
         </a:xfrm>
@@ -2859,8 +3455,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3722844" y="9178268"/>
-          <a:ext cx="3522949" cy="2168492"/>
+          <a:off x="3554756" y="9407055"/>
+          <a:ext cx="3368868" cy="2233859"/>
           <a:chOff x="3708769" y="9847102"/>
           <a:chExt cx="3506303" cy="2212883"/>
         </a:xfrm>
@@ -3051,8 +3647,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3511176" y="11653577"/>
-          <a:ext cx="3104403" cy="1817014"/>
+          <a:off x="3343088" y="11966408"/>
+          <a:ext cx="2950322" cy="1882382"/>
           <a:chOff x="3497101" y="12377899"/>
           <a:chExt cx="3087757" cy="1855856"/>
         </a:xfrm>
@@ -3388,7 +3984,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3818,8 +4414,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="569025" y="9879610"/>
-          <a:ext cx="11283867" cy="4706587"/>
+          <a:off x="552532" y="10007434"/>
+          <a:ext cx="10760198" cy="4780808"/>
           <a:chOff x="486557" y="9450779"/>
           <a:chExt cx="11283867" cy="4706587"/>
         </a:xfrm>
@@ -4202,6 +4798,347 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>218281</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>70970</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1087438" cy="1319322"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D77B1B90-8562-4EB3-B5B6-22F99336DD34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="218281" y="11631145"/>
+          <a:ext cx="1087438" cy="1319322"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>182562</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5203031" cy="1393448"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E183E8C9-E9C5-4507-8A79-9B52BAFC48A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="182562" y="14046201"/>
+          <a:ext cx="5203031" cy="1393448"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>496093</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>67469</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1452563" cy="493942"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE1DDDC-8735-47BA-A87E-285FD82143CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3391693" y="16313944"/>
+          <a:ext cx="1452563" cy="493942"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123031</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>246064</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3254375" cy="1743322"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A1B1303-92F7-465C-B16F-06FDE9453D55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="123031" y="16492539"/>
+          <a:ext cx="3254375" cy="1743322"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>115094</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1837531" cy="717550"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C25F60-7695-4958-9483-8CB2A865127B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="214313" y="18704719"/>
+          <a:ext cx="1837531" cy="717550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>829468</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>198438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>785812</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3969</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15DCBFD8-BF66-4FD1-A3F2-BFCFEB8E094D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2759868" y="16705263"/>
+          <a:ext cx="921544" cy="326231"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4483,22 +5420,22 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="20.5" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.11328125" customWidth="1"/>
+    <col min="3" max="3" width="6.33984375" customWidth="1"/>
+    <col min="4" max="4" width="3.76953125" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -4511,19 +5448,19 @@
         <v>2</v>
       </c>
       <c r="F1" s="4">
-        <v>44218</v>
+        <v>44756</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="1"/>
-      <c r="B2" s="23"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -4531,108 +5468,108 @@
       <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="26"/>
-    </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
+      <c r="H2" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="32"/>
+    </row>
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A3" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-    </row>
-    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+    </row>
+    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-    </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-    </row>
-    <row r="10" spans="1:9" ht="9.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+    </row>
+    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10" spans="1:9" ht="9.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="G11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="27"/>
-    </row>
-    <row r="12" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -4641,10 +5578,10 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A14" s="14">
         <v>1</v>
       </c>
@@ -4656,7 +5593,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>7</v>
@@ -4665,7 +5602,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
@@ -4675,7 +5612,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -4683,7 +5620,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4691,7 +5628,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -4699,7 +5636,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -4707,33 +5644,33 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A26" s="14">
         <v>2</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A27" s="2"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-    </row>
-    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="1">
       <c r="A28" s="2"/>
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
@@ -4744,7 +5681,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4755,7 +5692,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4766,7 +5703,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4777,7 +5714,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4788,7 +5725,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4799,191 +5736,191 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A34" s="14">
         <v>3</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-    </row>
-    <row r="47" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+    </row>
+    <row r="47" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A47" s="14">
         <v>4</v>
       </c>
-      <c r="B47" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B47" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.9">
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.9">
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.9">
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.9">
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.9">
       <c r="A62" s="14">
         <v>5</v>
       </c>
-      <c r="B62" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="20"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="20"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="20"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="20"/>
-      <c r="K64" s="20"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B62" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.9">
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="26"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.9">
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="26"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.9">
       <c r="B75" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A77" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A79" s="14" t="s">
         <v>24</v>
       </c>
@@ -4991,7 +5928,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A84" s="14" t="s">
         <v>25</v>
       </c>
@@ -5018,24 +5955,262 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F16710-7EF1-4AAC-8AAE-6D4C8E1D8883}">
+  <dimension ref="A2:I42"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.5" x14ac:dyDescent="0.9"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A2" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.75" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A4" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A6" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="10" spans="1:9" ht="37" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A10" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A12" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A14" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A18" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A22" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A23" s="25"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A24" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A35" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A42" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A35:I36"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A2:I3"/>
+    <mergeCell ref="A4:I5"/>
+    <mergeCell ref="A6:I7"/>
+    <mergeCell ref="A12:I13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039D2BED-4EAA-4D5E-BAE4-C8663D40581D}">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="20.5" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>68</v>
+      <c r="B1" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -5052,69 +6227,69 @@
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="33"/>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="1"/>
-      <c r="B2" s="23"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-    </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="G2" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+    </row>
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A3" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="15"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-    </row>
-    <row r="4" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+    </row>
+    <row r="4" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="15"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+    </row>
+    <row r="5" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="15"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-    </row>
-    <row r="6" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+    </row>
+    <row r="6" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -5124,34 +6299,34 @@
       <c r="G7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="30"/>
-    </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I7" s="42"/>
+    </row>
+    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A8" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
         <v>9</v>
@@ -5161,7 +6336,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -5171,7 +6346,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A13" s="14">
         <v>1</v>
       </c>
@@ -5183,7 +6358,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>7</v>
@@ -5192,7 +6367,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>14</v>
@@ -5202,7 +6377,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -5210,7 +6385,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -5218,7 +6393,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5226,7 +6401,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -5234,8 +6409,8 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="25" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -5246,33 +6421,33 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A26" s="14">
         <v>2</v>
       </c>
-      <c r="B26" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-    </row>
-    <row r="27" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A27" s="2"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-    </row>
-    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="1">
       <c r="A28" s="2"/>
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
@@ -5283,7 +6458,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -5294,7 +6469,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -5305,7 +6480,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -5316,7 +6491,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -5327,7 +6502,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -5338,170 +6513,170 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A34" s="14">
         <v>3</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A37" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-    </row>
-    <row r="43" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+    </row>
+    <row r="43" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A43" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-    </row>
-    <row r="53" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+    </row>
+    <row r="53" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A53" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-    </row>
-    <row r="56" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+    </row>
+    <row r="56" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A56" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B56" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="28"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="28"/>
-      <c r="I57" s="28"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="28"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="28"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B56" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A59" s="14">
         <v>4</v>
       </c>
@@ -5509,32 +6684,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A60" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A73" s="14" t="s">
         <v>34</v>
       </c>
@@ -5542,57 +6717,57 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.9">
       <c r="C74" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A83" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B83" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C83" s="28"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="28"/>
-      <c r="F83" s="28"/>
-      <c r="G83" s="28"/>
-      <c r="H83" s="28"/>
-      <c r="I83" s="28"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B84" s="28"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="28"/>
-      <c r="E84" s="28"/>
-      <c r="F84" s="28"/>
-      <c r="G84" s="28"/>
-      <c r="H84" s="28"/>
-      <c r="I84" s="28"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B85" s="28"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="28"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="28"/>
-      <c r="H85" s="28"/>
-      <c r="I85" s="28"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="28"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B83" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="43"/>
+      <c r="D83" s="43"/>
+      <c r="E83" s="43"/>
+      <c r="F83" s="43"/>
+      <c r="G83" s="43"/>
+      <c r="H83" s="43"/>
+      <c r="I83" s="43"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B84" s="43"/>
+      <c r="C84" s="43"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="43"/>
+      <c r="F84" s="43"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="43"/>
+      <c r="I84" s="43"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B85" s="43"/>
+      <c r="C85" s="43"/>
+      <c r="D85" s="43"/>
+      <c r="E85" s="43"/>
+      <c r="F85" s="43"/>
+      <c r="G85" s="43"/>
+      <c r="H85" s="43"/>
+      <c r="I85" s="43"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B86" s="43"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
+      <c r="G86" s="43"/>
+      <c r="H86" s="43"/>
+      <c r="I86" s="43"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A87" s="14">
         <v>5</v>
       </c>
@@ -5600,130 +6775,130 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.9">
       <c r="A99" s="14">
         <v>6</v>
       </c>
       <c r="B99" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.9">
       <c r="A106" s="14">
         <v>7</v>
       </c>
-      <c r="B106" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C106" s="20"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="20"/>
-      <c r="F106" s="20"/>
-      <c r="G106" s="20"/>
-      <c r="H106" s="20"/>
-      <c r="I106" s="20"/>
-      <c r="J106" s="20"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B107" s="20"/>
-      <c r="C107" s="20"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="20"/>
-      <c r="H107" s="20"/>
-      <c r="I107" s="20"/>
-      <c r="J107" s="20"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B108" s="20"/>
-      <c r="C108" s="20"/>
-      <c r="D108" s="20"/>
-      <c r="E108" s="20"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="20"/>
-      <c r="H108" s="20"/>
-      <c r="I108" s="20"/>
-      <c r="J108" s="20"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B109" s="20"/>
-      <c r="C109" s="20"/>
-      <c r="D109" s="20"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="20"/>
-      <c r="H109" s="20"/>
-      <c r="I109" s="20"/>
-      <c r="J109" s="20"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B110" s="20"/>
-      <c r="C110" s="20"/>
-      <c r="D110" s="20"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="20"/>
-      <c r="I110" s="20"/>
-      <c r="J110" s="20"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B106" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C106" s="26"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
+      <c r="F106" s="26"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="26"/>
+      <c r="I106" s="26"/>
+      <c r="J106" s="26"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.9">
+      <c r="B107" s="26"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="26"/>
+      <c r="G107" s="26"/>
+      <c r="H107" s="26"/>
+      <c r="I107" s="26"/>
+      <c r="J107" s="26"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.9">
+      <c r="B108" s="26"/>
+      <c r="C108" s="26"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+      <c r="F108" s="26"/>
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="26"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.9">
+      <c r="B109" s="26"/>
+      <c r="C109" s="26"/>
+      <c r="D109" s="26"/>
+      <c r="E109" s="26"/>
+      <c r="F109" s="26"/>
+      <c r="G109" s="26"/>
+      <c r="H109" s="26"/>
+      <c r="I109" s="26"/>
+      <c r="J109" s="26"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.9">
+      <c r="B110" s="26"/>
+      <c r="C110" s="26"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="26"/>
+      <c r="F110" s="26"/>
+      <c r="G110" s="26"/>
+      <c r="H110" s="26"/>
+      <c r="I110" s="26"/>
+      <c r="J110" s="26"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A114" s="14">
         <v>8</v>
       </c>
       <c r="B114" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.9">
+      <c r="B119" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B119" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B106:J110"/>
+    <mergeCell ref="B60:I61"/>
+    <mergeCell ref="B83:I86"/>
+    <mergeCell ref="B53:I54"/>
+    <mergeCell ref="B56:I58"/>
+    <mergeCell ref="B43:D51"/>
+    <mergeCell ref="B26:I27"/>
+    <mergeCell ref="H7:I9"/>
+    <mergeCell ref="B34:H35"/>
+    <mergeCell ref="B37:D41"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A3:D6"/>
     <mergeCell ref="G2:I6"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A8:F9"/>
-    <mergeCell ref="B43:D51"/>
-    <mergeCell ref="B26:I27"/>
-    <mergeCell ref="H7:I9"/>
-    <mergeCell ref="B34:H35"/>
-    <mergeCell ref="B37:D41"/>
-    <mergeCell ref="B106:J110"/>
-    <mergeCell ref="B60:I61"/>
-    <mergeCell ref="B83:I86"/>
-    <mergeCell ref="B53:I54"/>
-    <mergeCell ref="B56:I58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEB2658-D906-42E6-854D-E17B81D5C237}">
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView topLeftCell="A85" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="20.5" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.609375" customWidth="1"/>
+    <col min="1" max="1" width="4.5390625" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -5740,12 +6915,12 @@
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="33"/>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="1"/>
       <c r="B2" s="16"/>
       <c r="C2" s="2"/>
@@ -5754,46 +6929,46 @@
       <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-    </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="31" t="s">
+      <c r="G2" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+    </row>
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A3" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-    </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+    </row>
+    <row r="5" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+    </row>
+    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
@@ -5802,43 +6977,43 @@
       <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="30"/>
-    </row>
-    <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
+      <c r="H6" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="42"/>
+    </row>
+    <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A7" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="19"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-    </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+    </row>
+    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="19"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.9">
       <c r="F9" s="17"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A11" s="2"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
@@ -5848,10 +7023,10 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -5864,69 +7039,69 @@
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.9">
       <c r="A13" s="14">
         <v>1</v>
       </c>
-      <c r="B13" s="35" t="s">
-        <v>71</v>
+      <c r="B13" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B14" s="35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="B14" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A22" s="14">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A36" s="14">
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A38" s="14">
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A57" s="14">
         <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A67" s="14">
         <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.9">
       <c r="A75" s="14">
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -5943,7 +7118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D09C306-5FA0-4678-AE18-A50D1EA02C6F}">
   <sheetPr>
     <tabColor theme="3" tint="0.79998168889431442"/>
@@ -5954,60 +7129,60 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="20.5" x14ac:dyDescent="0.9"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A5" s="11"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A8" s="11"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A10" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -6019,4 +7194,183 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC50D0CA-9DAD-42B4-B8D1-4A1ED6855B6D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.5" x14ac:dyDescent="0.9"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B078194A-2B4F-419C-BD02-5DE55DAE7D58}">
+  <dimension ref="A2:I35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.5" x14ac:dyDescent="0.9"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A2" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A3" s="21"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A6" s="21"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A8" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A11" s="45"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A18" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A20" s="45"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A33" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A34" s="45"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.9">
+      <c r="A35" s="45"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A8:I9"/>
+    <mergeCell ref="A10:I11"/>
+    <mergeCell ref="A18:I20"/>
+    <mergeCell ref="A33:I35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>